<commit_message>
Add torch accelerating and fix bugs。
</commit_message>
<xml_diff>
--- a/memristordata/retention_loss.xlsx
+++ b/memristordata/retention_loss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LAB2023\20230518_I-t_fit\20230518_I-t_fit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repository\mem-brain-bindsnet\memristordata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71642F22-1826-4E27-B9C2-C417F169C174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58650835-E772-4303-8B96-6FDC9C15ABCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3560" yWindow="5700" windowWidth="28800" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,6 +40,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,9 +68,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -348,3214 +355,3217 @@
   <dimension ref="A1:B400"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="8.6640625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
         <v>0.4</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>1.3300000000000001E-10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
         <v>0.8</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>1.2299999999999999E-10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>1.2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>1.2E-10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>1.6</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>1.1700000000000001E-10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>1.16E-10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>2.4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>1.15E-10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>2.8</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>1.15E-10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>3.2</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>1.15E-10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>3.6</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>1.15E-10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
         <v>4</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>1.1399999999999999E-10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>1.1399999999999999E-10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
         <v>4.8</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>1.15E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>5.2</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>1.12E-10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A14">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
         <v>5.6</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>1.11E-10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>6</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="2">
         <v>1.0999999999999999E-10</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A16">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>6.4</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="2">
         <v>1.0999999999999999E-10</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>6.8</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="2">
         <v>1.09E-10</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>7.2</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>1.11E-10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
         <v>7.6</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>1.12E-10</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
         <v>8</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>1.09E-10</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
         <v>8.4</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>1.0700000000000001E-10</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A22">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>8.8000000000000007</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22" s="2">
         <v>1.08E-10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A23">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>1.08E-10</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A24">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>9.6</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>1.0700000000000001E-10</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
         <v>10</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>1.05E-10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A26">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>10.4</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>1.05E-10</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A27">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
         <v>10.8</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>1.06E-10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A28">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
         <v>11.2</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>1.05E-10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A29">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
         <v>11.6</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>1.0300000000000001E-10</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A30">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
         <v>12</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30" s="2">
         <v>1.0300000000000001E-10</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A31">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
         <v>12.4</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>1.04E-10</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A32">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>12.8</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>1.02E-10</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A33">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
         <v>13.2</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>1.01E-10</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A34">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>13.6</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>1.01E-10</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
         <v>14</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>1.0300000000000001E-10</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A36">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
         <v>14.4</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="2">
         <v>1.02E-10</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A37">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>14.8</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>1.02E-10</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A38">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
         <v>15.2</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>9.8199999999999994E-11</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A39">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
         <v>15.6</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>9.8499999999999996E-11</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A40">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
         <v>16</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40" s="2">
         <v>9.8499999999999996E-11</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A41">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
         <v>16.399999999999999</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>9.8799999999999997E-11</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A42">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
         <v>16.8</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>9.7300000000000003E-11</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A43">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
         <v>17.2</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>9.6099999999999996E-11</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A44">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
         <v>17.600000000000001</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>9.6800000000000004E-11</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
         <v>18</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45" s="2">
         <v>9.7300000000000003E-11</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A46">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
         <v>18.399999999999999</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>9.5299999999999997E-11</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A47">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
         <v>18.8</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47" s="2">
         <v>9.51E-11</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A48">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
         <v>19.2</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48" s="2">
         <v>9.4999999999999995E-11</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A49">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
         <v>19.600000000000001</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>9.4900000000000003E-11</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A50">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
         <v>20</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50" s="2">
         <v>9.4199999999999995E-11</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A51">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
         <v>20.399999999999999</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>9.2200000000000002E-11</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A52">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
         <v>20.8</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52" s="2">
         <v>9.27E-11</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A53">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
         <v>21.2</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53" s="2">
         <v>9.3600000000000005E-11</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A54">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
         <v>21.6</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="2">
         <v>9.2899999999999997E-11</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A55">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
         <v>22</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>9.1599999999999999E-11</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A56">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
         <v>22.4</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <v>9.1400000000000002E-11</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A57">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
         <v>22.8</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57" s="2">
         <v>9.1900000000000001E-11</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A58">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
         <v>23.2</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58" s="2">
         <v>9.1700000000000004E-11</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A59">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
         <v>23.6</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59" s="2">
         <v>9.1299999999999997E-11</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A60">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
         <v>24</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="2">
         <v>9.0100000000000004E-11</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A61">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
         <v>24.4</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61" s="2">
         <v>8.9899999999999995E-11</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A62">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
         <v>24.8</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="2">
         <v>8.92E-11</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A63">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
         <v>25.2</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63" s="2">
         <v>8.9099999999999995E-11</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A64">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
         <v>25.6</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64" s="2">
         <v>8.8800000000000006E-11</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A65">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
         <v>26</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65" s="2">
         <v>8.8099999999999998E-11</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A66">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
         <v>26.4</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66" s="2">
         <v>8.7900000000000001E-11</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A67">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
         <v>26.8</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67" s="2">
         <v>8.7100000000000002E-11</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A68">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
         <v>27.2</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="2">
         <v>8.8500000000000005E-11</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A69">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
         <v>27.6</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="2">
         <v>8.7700000000000005E-11</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A70">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
         <v>28</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="2">
         <v>8.6900000000000005E-11</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A71">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
         <v>28.4</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="2">
         <v>8.5699999999999999E-11</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A72">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
         <v>28.8</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72" s="2">
         <v>8.52E-11</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A73">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
         <v>29.2</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="2">
         <v>8.5500000000000002E-11</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A74">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
         <v>29.6</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="2">
         <v>8.52E-11</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A75">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
         <v>30</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="2">
         <v>8.3499999999999996E-11</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A76">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
         <v>30.4</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76" s="2">
         <v>8.2800000000000001E-11</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A77">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
         <v>30.8</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="2">
         <v>8.2499999999999999E-11</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A78">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
         <v>31.2</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="2">
         <v>8.0700000000000003E-11</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A79">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
         <v>31.6</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="2">
         <v>8.2800000000000001E-11</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A80">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
         <v>32</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80" s="2">
         <v>8.2199999999999998E-11</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A81">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
         <v>32.4</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81" s="2">
         <v>8.1800000000000004E-11</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A82">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
         <v>32.799999999999997</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="2">
         <v>8.1099999999999997E-11</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A83">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
         <v>33.200000000000003</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="2">
         <v>8.1200000000000001E-11</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A84">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
         <v>33.6</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84" s="2">
         <v>8.2300000000000003E-11</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A85">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
         <v>34</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85" s="2">
         <v>8.1200000000000001E-11</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A86">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
         <v>34.4</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86" s="2">
         <v>7.9900000000000003E-11</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A87">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
         <v>34.799999999999997</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87" s="2">
         <v>8.01E-11</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A88">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
         <v>35.200000000000003</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88" s="2">
         <v>8.01E-11</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A89">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
         <v>35.6</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89" s="2">
         <v>7.9799999999999998E-11</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A90">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
         <v>36</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90" s="2">
         <v>8.01E-11</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A91">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
         <v>36.4</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91" s="2">
         <v>7.8300000000000004E-11</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A92">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
         <v>36.799999999999997</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="2">
         <v>7.7000000000000006E-11</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A93">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
         <v>37.200000000000003</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93" s="2">
         <v>7.8600000000000005E-11</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A94">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
         <v>37.6</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94" s="2">
         <v>7.8699999999999997E-11</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A95">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
         <v>38</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95" s="2">
         <v>7.8399999999999996E-11</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A96">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
         <v>38.4</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="2">
         <v>7.7800000000000005E-11</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A97">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
         <v>38.799999999999997</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97" s="2">
         <v>7.6900000000000001E-11</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A98">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
         <v>39.200000000000003</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98" s="2">
         <v>7.7299999999999994E-11</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A99">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
         <v>39.6</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="2">
         <v>7.7299999999999994E-11</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A100">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
         <v>40</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100" s="2">
         <v>7.7800000000000005E-11</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A101">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
         <v>40.4</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101" s="2">
         <v>7.7200000000000002E-11</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A102">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="1">
         <v>40.799999999999997</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102" s="2">
         <v>7.5799999999999999E-11</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A103">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
         <v>41.2</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103" s="2">
         <v>7.34E-11</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A104">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="1">
         <v>41.6</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104" s="2">
         <v>7.34E-11</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A105">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="1">
         <v>42</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105" s="2">
         <v>7.4399999999999996E-11</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A106">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
         <v>42.4</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106" s="2">
         <v>7.5E-11</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A107">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
         <v>42.8</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107" s="2">
         <v>7.3099999999999998E-11</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A108">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
         <v>43.2</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108" s="2">
         <v>7.3700000000000001E-11</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A109">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
         <v>43.6</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109" s="2">
         <v>7.5E-11</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A110">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
         <v>44</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110" s="2">
         <v>7.4000000000000003E-11</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A111">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
         <v>44.4</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111" s="2">
         <v>7.1699999999999995E-11</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A112">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
         <v>44.8</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112" s="2">
         <v>7.1300000000000002E-11</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A113">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
         <v>45.2</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113" s="2">
         <v>7.3599999999999997E-11</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A114">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
         <v>45.6</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114" s="2">
         <v>7.4099999999999995E-11</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A115">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
         <v>46</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115" s="2">
         <v>7.1100000000000005E-11</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A116">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
         <v>46.4</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116" s="2">
         <v>7.2799999999999997E-11</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A117">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
         <v>46.8</v>
       </c>
-      <c r="B117" s="1">
+      <c r="B117" s="2">
         <v>7.26E-11</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A118">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
         <v>47.2</v>
       </c>
-      <c r="B118" s="1">
+      <c r="B118" s="2">
         <v>7.26E-11</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A119">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
         <v>47.6</v>
       </c>
-      <c r="B119" s="1">
+      <c r="B119" s="2">
         <v>7.1399999999999994E-11</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A120">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
         <v>48</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B120" s="2">
         <v>7.0099999999999996E-11</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A121">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
         <v>48.4</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B121" s="2">
         <v>6.9500000000000006E-11</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A122">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
         <v>48.8</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122" s="2">
         <v>7.0500000000000002E-11</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A123">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
         <v>49.2</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123" s="2">
         <v>7.0200000000000001E-11</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A124">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
         <v>49.6</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124" s="2">
         <v>6.9400000000000001E-11</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A125">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
         <v>50</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B125" s="2">
         <v>6.8299999999999999E-11</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A126">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" s="1">
         <v>50.4</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B126" s="2">
         <v>7.0000000000000004E-11</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A127">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="1">
         <v>50.8</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B127" s="2">
         <v>6.8900000000000002E-11</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A128">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" s="1">
         <v>51.2</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B128" s="2">
         <v>6.7800000000000001E-11</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A129">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="1">
         <v>51.6</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B129" s="2">
         <v>6.7000000000000001E-11</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A130">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" s="1">
         <v>52</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B130" s="2">
         <v>6.67E-11</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A131">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="1">
         <v>52.4</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B131" s="2">
         <v>6.6500000000000003E-11</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A132">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="1">
         <v>52.8</v>
       </c>
-      <c r="B132" s="1">
+      <c r="B132" s="2">
         <v>6.6899999999999996E-11</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A133">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" s="1">
         <v>53.2</v>
       </c>
-      <c r="B133" s="1">
+      <c r="B133" s="2">
         <v>6.67E-11</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A134">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="1">
         <v>53.6</v>
       </c>
-      <c r="B134" s="1">
+      <c r="B134" s="2">
         <v>6.5799999999999995E-11</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A135">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" s="1">
         <v>54</v>
       </c>
-      <c r="B135" s="1">
+      <c r="B135" s="2">
         <v>6.5700000000000003E-11</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A136">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" s="1">
         <v>54.4</v>
       </c>
-      <c r="B136" s="1">
+      <c r="B136" s="2">
         <v>6.5299999999999997E-11</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A137">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" s="1">
         <v>54.8</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137" s="2">
         <v>6.4900000000000003E-11</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A138">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="1">
         <v>55.2</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138" s="2">
         <v>6.4999999999999995E-11</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A139">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" s="1">
         <v>55.6</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139" s="2">
         <v>6.3899999999999994E-11</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A140">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="1">
         <v>56</v>
       </c>
-      <c r="B140" s="1">
+      <c r="B140" s="2">
         <v>6.35E-11</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A141">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="1">
         <v>56.4</v>
       </c>
-      <c r="B141" s="1">
+      <c r="B141" s="2">
         <v>6.3899999999999994E-11</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A142">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="1">
         <v>56.8</v>
       </c>
-      <c r="B142" s="1">
+      <c r="B142" s="2">
         <v>6.3600000000000005E-11</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A143">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="1">
         <v>57.2</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143" s="2">
         <v>6.2899999999999997E-11</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A144">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="1">
         <v>57.6</v>
       </c>
-      <c r="B144" s="1">
+      <c r="B144" s="2">
         <v>6.2299999999999994E-11</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A145">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" s="1">
         <v>58</v>
       </c>
-      <c r="B145" s="1">
+      <c r="B145" s="2">
         <v>6.3199999999999999E-11</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A146">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" s="1">
         <v>58.4</v>
       </c>
-      <c r="B146" s="1">
+      <c r="B146" s="2">
         <v>6.1599999999999999E-11</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A147">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" s="1">
         <v>58.8</v>
       </c>
-      <c r="B147" s="1">
+      <c r="B147" s="2">
         <v>6.2899999999999997E-11</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A148">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" s="1">
         <v>59.2</v>
       </c>
-      <c r="B148" s="1">
+      <c r="B148" s="2">
         <v>6.1799999999999996E-11</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A149">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" s="1">
         <v>59.6</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="2">
         <v>6.0600000000000003E-11</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A150">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" s="1">
         <v>60</v>
       </c>
-      <c r="B150" s="1">
+      <c r="B150" s="2">
         <v>6.0300000000000001E-11</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A151">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" s="1">
         <v>60.4</v>
       </c>
-      <c r="B151" s="1">
+      <c r="B151" s="2">
         <v>6.1499999999999994E-11</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A152">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" s="1">
         <v>60.8</v>
       </c>
-      <c r="B152" s="1">
+      <c r="B152" s="2">
         <v>6.1400000000000003E-11</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A153">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="1">
         <v>61.2</v>
       </c>
-      <c r="B153" s="1">
+      <c r="B153" s="2">
         <v>6.0799999999999999E-11</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A154">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" s="1">
         <v>61.6</v>
       </c>
-      <c r="B154" s="1">
+      <c r="B154" s="2">
         <v>5.9500000000000001E-11</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A155">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" s="1">
         <v>62</v>
       </c>
-      <c r="B155" s="1">
+      <c r="B155" s="2">
         <v>5.9300000000000005E-11</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A156">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" s="1">
         <v>62.4</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156" s="2">
         <v>6.0799999999999999E-11</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A157">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" s="1">
         <v>62.8</v>
       </c>
-      <c r="B157" s="1">
+      <c r="B157" s="2">
         <v>6.0499999999999998E-11</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A158">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" s="1">
         <v>63.2</v>
       </c>
-      <c r="B158" s="1">
+      <c r="B158" s="2">
         <v>5.8299999999999995E-11</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A159">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" s="1">
         <v>63.6</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159" s="2">
         <v>5.7900000000000002E-11</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A160">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" s="1">
         <v>64</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160" s="2">
         <v>5.7399999999999997E-11</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A161">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" s="1">
         <v>64.400000000000006</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161" s="2">
         <v>5.8099999999999998E-11</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A162">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" s="1">
         <v>64.8</v>
       </c>
-      <c r="B162" s="1">
+      <c r="B162" s="2">
         <v>5.8899999999999998E-11</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A163">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" s="1">
         <v>65.2</v>
       </c>
-      <c r="B163" s="1">
+      <c r="B163" s="2">
         <v>5.7399999999999997E-11</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A164">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" s="1">
         <v>65.599999999999994</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164" s="2">
         <v>5.6899999999999999E-11</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A165">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" s="1">
         <v>66</v>
       </c>
-      <c r="B165" s="1">
+      <c r="B165" s="2">
         <v>5.6599999999999997E-11</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A166">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" s="1">
         <v>66.400000000000006</v>
       </c>
-      <c r="B166" s="1">
+      <c r="B166" s="2">
         <v>5.7299999999999999E-11</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A167">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" s="1">
         <v>66.8</v>
       </c>
-      <c r="B167" s="1">
+      <c r="B167" s="2">
         <v>5.6499999999999999E-11</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A168">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" s="1">
         <v>67.2</v>
       </c>
-      <c r="B168" s="1">
+      <c r="B168" s="2">
         <v>5.6E-11</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A169">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" s="1">
         <v>67.599999999999994</v>
       </c>
-      <c r="B169" s="1">
+      <c r="B169" s="2">
         <v>5.4599999999999998E-11</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A170">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" s="1">
         <v>68</v>
       </c>
-      <c r="B170" s="1">
+      <c r="B170" s="2">
         <v>5.6499999999999999E-11</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A171">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A171" s="1">
         <v>68.400000000000006</v>
       </c>
-      <c r="B171" s="1">
+      <c r="B171" s="2">
         <v>5.6999999999999997E-11</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A172">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" s="1">
         <v>68.8</v>
       </c>
-      <c r="B172" s="1">
+      <c r="B172" s="2">
         <v>5.5600000000000001E-11</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A173">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" s="1">
         <v>69.2</v>
       </c>
-      <c r="B173" s="1">
+      <c r="B173" s="2">
         <v>5.5200000000000001E-11</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A174">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" s="1">
         <v>69.599999999999994</v>
       </c>
-      <c r="B174" s="1">
+      <c r="B174" s="2">
         <v>5.4300000000000002E-11</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A175">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" s="1">
         <v>70</v>
       </c>
-      <c r="B175" s="1">
+      <c r="B175" s="2">
         <v>5.5299999999999999E-11</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A176">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" s="1">
         <v>70.400000000000006</v>
       </c>
-      <c r="B176" s="1">
+      <c r="B176" s="2">
         <v>5.4000000000000001E-11</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A177">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" s="1">
         <v>70.8</v>
       </c>
-      <c r="B177" s="1">
+      <c r="B177" s="2">
         <v>5.4499999999999999E-11</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A178">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" s="1">
         <v>71.2</v>
       </c>
-      <c r="B178" s="1">
+      <c r="B178" s="2">
         <v>5.25E-11</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A179">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" s="1">
         <v>71.599999999999994</v>
       </c>
-      <c r="B179" s="1">
+      <c r="B179" s="2">
         <v>5.3600000000000001E-11</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A180">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" s="1">
         <v>72</v>
       </c>
-      <c r="B180" s="1">
+      <c r="B180" s="2">
         <v>5.4099999999999999E-11</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A181">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" s="1">
         <v>72.400000000000006</v>
       </c>
-      <c r="B181" s="1">
+      <c r="B181" s="2">
         <v>5.4099999999999999E-11</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A182">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" s="1">
         <v>72.8</v>
       </c>
-      <c r="B182" s="1">
+      <c r="B182" s="2">
         <v>5.1100000000000003E-11</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A183">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" s="1">
         <v>73.2</v>
       </c>
-      <c r="B183" s="1">
+      <c r="B183" s="2">
         <v>5.2300000000000003E-11</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A184">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" s="1">
         <v>73.599999999999994</v>
       </c>
-      <c r="B184" s="1">
+      <c r="B184" s="2">
         <v>5.3600000000000001E-11</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A185">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" s="1">
         <v>74</v>
       </c>
-      <c r="B185" s="1">
+      <c r="B185" s="2">
         <v>5.1200000000000002E-11</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A186">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" s="1">
         <v>74.400000000000006</v>
       </c>
-      <c r="B186" s="1">
+      <c r="B186" s="2">
         <v>4.9899999999999997E-11</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A187">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" s="1">
         <v>74.8</v>
       </c>
-      <c r="B187" s="1">
+      <c r="B187" s="2">
         <v>4.9600000000000002E-11</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A188">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188" s="1">
         <v>75.2</v>
       </c>
-      <c r="B188" s="1">
+      <c r="B188" s="2">
         <v>5.0400000000000002E-11</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A189">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189" s="1">
         <v>75.599999999999994</v>
       </c>
-      <c r="B189" s="1">
+      <c r="B189" s="2">
         <v>5.1399999999999998E-11</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A190">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" s="1">
         <v>76</v>
       </c>
-      <c r="B190" s="1">
+      <c r="B190" s="2">
         <v>5.1100000000000003E-11</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A191">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" s="1">
         <v>76.400000000000006</v>
       </c>
-      <c r="B191" s="1">
+      <c r="B191" s="2">
         <v>4.9099999999999997E-11</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A192">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" s="1">
         <v>76.8</v>
       </c>
-      <c r="B192" s="1">
+      <c r="B192" s="2">
         <v>4.9799999999999999E-11</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A193">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193" s="1">
         <v>77.2</v>
       </c>
-      <c r="B193" s="1">
+      <c r="B193" s="2">
         <v>5.0199999999999999E-11</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A194">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194" s="1">
         <v>77.599999999999994</v>
       </c>
-      <c r="B194" s="1">
+      <c r="B194" s="2">
         <v>4.9799999999999999E-11</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A195">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" s="1">
         <v>78</v>
       </c>
-      <c r="B195" s="1">
+      <c r="B195" s="2">
         <v>4.8800000000000002E-11</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A196">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" s="1">
         <v>78.400000000000006</v>
       </c>
-      <c r="B196" s="1">
+      <c r="B196" s="2">
         <v>4.9399999999999999E-11</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A197">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" s="1">
         <v>78.8</v>
       </c>
-      <c r="B197" s="1">
+      <c r="B197" s="2">
         <v>4.6699999999999998E-11</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A198">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" s="1">
         <v>79.2</v>
       </c>
-      <c r="B198" s="1">
+      <c r="B198" s="2">
         <v>4.7399999999999999E-11</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A199">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199" s="1">
         <v>79.599999999999994</v>
       </c>
-      <c r="B199" s="1">
+      <c r="B199" s="2">
         <v>4.8400000000000002E-11</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A200">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" s="1">
         <v>80</v>
       </c>
-      <c r="B200" s="1">
+      <c r="B200" s="2">
         <v>4.8100000000000001E-11</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A201">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201" s="1">
         <v>80.400000000000006</v>
       </c>
-      <c r="B201" s="1">
+      <c r="B201" s="2">
         <v>4.9600000000000002E-11</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A202">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202" s="1">
         <v>80.8</v>
       </c>
-      <c r="B202" s="1">
+      <c r="B202" s="2">
         <v>4.5700000000000001E-11</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A203">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203" s="1">
         <v>81.2</v>
       </c>
-      <c r="B203" s="1">
+      <c r="B203" s="2">
         <v>4.5300000000000001E-11</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A204">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204" s="1">
         <v>81.599999999999994</v>
       </c>
-      <c r="B204" s="1">
+      <c r="B204" s="2">
         <v>4.7099999999999998E-11</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A205">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205" s="1">
         <v>82</v>
       </c>
-      <c r="B205" s="1">
+      <c r="B205" s="2">
         <v>4.6999999999999999E-11</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A206">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206" s="1">
         <v>82.4</v>
       </c>
-      <c r="B206" s="1">
+      <c r="B206" s="2">
         <v>4.58E-11</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A207">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" s="1">
         <v>82.8</v>
       </c>
-      <c r="B207" s="1">
+      <c r="B207" s="2">
         <v>4.5899999999999998E-11</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A208">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" s="1">
         <v>83.2</v>
       </c>
-      <c r="B208" s="1">
+      <c r="B208" s="2">
         <v>4.5600000000000003E-11</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A209">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209" s="1">
         <v>83.6</v>
       </c>
-      <c r="B209" s="1">
+      <c r="B209" s="2">
         <v>4.4900000000000001E-11</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A210">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" s="1">
         <v>84</v>
       </c>
-      <c r="B210" s="1">
+      <c r="B210" s="2">
         <v>4.42E-11</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A211">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211" s="1">
         <v>84.4</v>
       </c>
-      <c r="B211" s="1">
+      <c r="B211" s="2">
         <v>4.4900000000000001E-11</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A212">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212" s="1">
         <v>84.8</v>
       </c>
-      <c r="B212" s="1">
+      <c r="B212" s="2">
         <v>4.4800000000000003E-11</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A213">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" s="1">
         <v>85.2</v>
       </c>
-      <c r="B213" s="1">
+      <c r="B213" s="2">
         <v>4.4100000000000002E-11</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A214">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" s="1">
         <v>85.6</v>
       </c>
-      <c r="B214" s="1">
+      <c r="B214" s="2">
         <v>4.4000000000000003E-11</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A215">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215" s="1">
         <v>86</v>
       </c>
-      <c r="B215" s="1">
+      <c r="B215" s="2">
         <v>4.5600000000000003E-11</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A216">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" s="1">
         <v>86.4</v>
       </c>
-      <c r="B216" s="1">
+      <c r="B216" s="2">
         <v>4.4000000000000003E-11</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A217">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A217" s="1">
         <v>86.8</v>
       </c>
-      <c r="B217" s="1">
+      <c r="B217" s="2">
         <v>4.3700000000000002E-11</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A218">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218" s="1">
         <v>87.2</v>
       </c>
-      <c r="B218" s="1">
+      <c r="B218" s="2">
         <v>4.2900000000000002E-11</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A219">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219" s="1">
         <v>87.6</v>
       </c>
-      <c r="B219" s="1">
+      <c r="B219" s="2">
         <v>4.22E-11</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A220">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A220" s="1">
         <v>88</v>
       </c>
-      <c r="B220" s="1">
+      <c r="B220" s="2">
         <v>4.34E-11</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A221">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221" s="1">
         <v>88.4</v>
       </c>
-      <c r="B221" s="1">
+      <c r="B221" s="2">
         <v>4.3E-11</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A222">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" s="1">
         <v>88.8</v>
       </c>
-      <c r="B222" s="1">
+      <c r="B222" s="2">
         <v>4.38E-11</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A223">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" s="1">
         <v>89.2</v>
       </c>
-      <c r="B223" s="1">
+      <c r="B223" s="2">
         <v>4.1000000000000001E-11</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A224">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224" s="1">
         <v>89.6</v>
       </c>
-      <c r="B224" s="1">
+      <c r="B224" s="2">
         <v>4.18E-11</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A225">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" s="1">
         <v>90</v>
       </c>
-      <c r="B225" s="1">
+      <c r="B225" s="2">
         <v>4.1999999999999997E-11</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A226">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" s="1">
         <v>90.4</v>
       </c>
-      <c r="B226" s="1">
+      <c r="B226" s="2">
         <v>4.1700000000000002E-11</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A227">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" s="1">
         <v>90.8</v>
       </c>
-      <c r="B227" s="1">
+      <c r="B227" s="2">
         <v>4.18E-11</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A228">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228" s="1">
         <v>91.2</v>
       </c>
-      <c r="B228" s="1">
+      <c r="B228" s="2">
         <v>4.0299999999999999E-11</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A229">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229" s="1">
         <v>91.6</v>
       </c>
-      <c r="B229" s="1">
+      <c r="B229" s="2">
         <v>3.9400000000000001E-11</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A230">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230" s="1">
         <v>92</v>
       </c>
-      <c r="B230" s="1">
+      <c r="B230" s="2">
         <v>4.0699999999999999E-11</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A231">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A231" s="1">
         <v>92.4</v>
       </c>
-      <c r="B231" s="1">
+      <c r="B231" s="2">
         <v>4.1499999999999999E-11</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A232">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A232" s="1">
         <v>92.8</v>
       </c>
-      <c r="B232" s="1">
+      <c r="B232" s="2">
         <v>4.0799999999999997E-11</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A233">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A233" s="1">
         <v>93.2</v>
       </c>
-      <c r="B233" s="1">
+      <c r="B233" s="2">
         <v>3.9400000000000001E-11</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A234">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A234" s="1">
         <v>93.6</v>
       </c>
-      <c r="B234" s="1">
+      <c r="B234" s="2">
         <v>3.9999999999999998E-11</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A235">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A235" s="1">
         <v>94</v>
       </c>
-      <c r="B235" s="1">
+      <c r="B235" s="2">
         <v>3.9999999999999998E-11</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A236">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236" s="1">
         <v>94.4</v>
       </c>
-      <c r="B236" s="1">
+      <c r="B236" s="2">
         <v>4.1599999999999997E-11</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A237">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237" s="1">
         <v>94.8</v>
       </c>
-      <c r="B237" s="1">
+      <c r="B237" s="2">
         <v>4.0900000000000002E-11</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A238">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A238" s="1">
         <v>95.2</v>
       </c>
-      <c r="B238" s="1">
+      <c r="B238" s="2">
         <v>3.8699999999999999E-11</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A239">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A239" s="1">
         <v>95.6</v>
       </c>
-      <c r="B239" s="1">
+      <c r="B239" s="2">
         <v>3.9300000000000003E-11</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A240">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A240" s="1">
         <v>96</v>
       </c>
-      <c r="B240" s="1">
+      <c r="B240" s="2">
         <v>3.8900000000000003E-11</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A241">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A241" s="1">
         <v>96.4</v>
       </c>
-      <c r="B241" s="1">
+      <c r="B241" s="2">
         <v>4.0200000000000001E-11</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A242">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A242" s="1">
         <v>96.8</v>
       </c>
-      <c r="B242" s="1">
+      <c r="B242" s="2">
         <v>3.9300000000000003E-11</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A243">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A243" s="1">
         <v>97.2</v>
       </c>
-      <c r="B243" s="1">
+      <c r="B243" s="2">
         <v>3.8200000000000001E-11</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A244">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A244" s="1">
         <v>97.6</v>
       </c>
-      <c r="B244" s="1">
+      <c r="B244" s="2">
         <v>3.8600000000000001E-11</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A245">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A245" s="1">
         <v>98</v>
       </c>
-      <c r="B245" s="1">
+      <c r="B245" s="2">
         <v>3.75E-11</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A246">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A246" s="1">
         <v>98.4</v>
       </c>
-      <c r="B246" s="1">
+      <c r="B246" s="2">
         <v>3.7599999999999998E-11</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A247">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A247" s="1">
         <v>98.8</v>
       </c>
-      <c r="B247" s="1">
+      <c r="B247" s="2">
         <v>3.8699999999999999E-11</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A248">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A248" s="1">
         <v>99.2</v>
       </c>
-      <c r="B248" s="1">
+      <c r="B248" s="2">
         <v>3.79E-11</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A249">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A249" s="1">
         <v>99.6</v>
       </c>
-      <c r="B249" s="1">
+      <c r="B249" s="2">
         <v>3.6600000000000002E-11</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A250">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A250" s="1">
         <v>100</v>
       </c>
-      <c r="B250" s="1">
+      <c r="B250" s="2">
         <v>3.5999999999999998E-11</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A251">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A251" s="1">
         <v>100.4</v>
       </c>
-      <c r="B251" s="1">
+      <c r="B251" s="2">
         <v>3.6600000000000002E-11</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A252">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A252" s="1">
         <v>100.8</v>
       </c>
-      <c r="B252" s="1">
+      <c r="B252" s="2">
         <v>3.6799999999999998E-11</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A253">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A253" s="1">
         <v>101.2</v>
       </c>
-      <c r="B253" s="1">
+      <c r="B253" s="2">
         <v>3.6900000000000003E-11</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A254">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A254" s="1">
         <v>101.6</v>
       </c>
-      <c r="B254" s="1">
+      <c r="B254" s="2">
         <v>3.6500000000000003E-11</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A255">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A255" s="1">
         <v>102</v>
       </c>
-      <c r="B255" s="1">
+      <c r="B255" s="2">
         <v>3.47E-11</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A256">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A256" s="1">
         <v>102.4</v>
       </c>
-      <c r="B256" s="1">
+      <c r="B256" s="2">
         <v>3.5199999999999999E-11</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A257">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A257" s="1">
         <v>102.8</v>
       </c>
-      <c r="B257" s="1">
+      <c r="B257" s="2">
         <v>3.5699999999999997E-11</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A258">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258" s="1">
         <v>103.2</v>
       </c>
-      <c r="B258" s="1">
+      <c r="B258" s="2">
         <v>3.55E-11</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A259">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259" s="1">
         <v>103.6</v>
       </c>
-      <c r="B259" s="1">
+      <c r="B259" s="2">
         <v>3.51E-11</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A260">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260" s="1">
         <v>104</v>
       </c>
-      <c r="B260" s="1">
+      <c r="B260" s="2">
         <v>3.3100000000000001E-11</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A261">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261" s="1">
         <v>104.4</v>
       </c>
-      <c r="B261" s="1">
+      <c r="B261" s="2">
         <v>3.2499999999999998E-11</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A262">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262" s="1">
         <v>104.8</v>
       </c>
-      <c r="B262" s="1">
+      <c r="B262" s="2">
         <v>3.1999999999999999E-11</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A263">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263" s="1">
         <v>105.2</v>
       </c>
-      <c r="B263" s="1">
+      <c r="B263" s="2">
         <v>3.3500000000000001E-11</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A264">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264" s="1">
         <v>105.6</v>
       </c>
-      <c r="B264" s="1">
+      <c r="B264" s="2">
         <v>3.43E-11</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A265">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265" s="1">
         <v>106</v>
       </c>
-      <c r="B265" s="1">
+      <c r="B265" s="2">
         <v>3.3199999999999999E-11</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A266">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266" s="1">
         <v>106.4</v>
       </c>
-      <c r="B266" s="1">
+      <c r="B266" s="2">
         <v>3.12E-11</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A267">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267" s="1">
         <v>106.8</v>
       </c>
-      <c r="B267" s="1">
+      <c r="B267" s="2">
         <v>3.0899999999999998E-11</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A268">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268" s="1">
         <v>107.2</v>
       </c>
-      <c r="B268" s="1">
+      <c r="B268" s="2">
         <v>3.1599999999999999E-11</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A269">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269" s="1">
         <v>107.6</v>
       </c>
-      <c r="B269" s="1">
+      <c r="B269" s="2">
         <v>3.1699999999999998E-11</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A270">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270" s="1">
         <v>108</v>
       </c>
-      <c r="B270" s="1">
+      <c r="B270" s="2">
         <v>3.2399999999999999E-11</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A271">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271" s="1">
         <v>108.4</v>
       </c>
-      <c r="B271" s="1">
+      <c r="B271" s="2">
         <v>3.2799999999999999E-11</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A272">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272" s="1">
         <v>108.8</v>
       </c>
-      <c r="B272" s="1">
+      <c r="B272" s="2">
         <v>3.0899999999999998E-11</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A273">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A273" s="1">
         <v>109.2</v>
       </c>
-      <c r="B273" s="1">
+      <c r="B273" s="2">
         <v>3.0099999999999998E-11</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A274">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A274" s="1">
         <v>109.6</v>
       </c>
-      <c r="B274" s="1">
+      <c r="B274" s="2">
         <v>3.1000000000000003E-11</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A275">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A275" s="1">
         <v>110</v>
       </c>
-      <c r="B275" s="1">
+      <c r="B275" s="2">
         <v>3.1500000000000001E-11</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A276">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A276" s="1">
         <v>110.4</v>
       </c>
-      <c r="B276" s="1">
+      <c r="B276" s="2">
         <v>3.1999999999999999E-11</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A277">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A277" s="1">
         <v>110.8</v>
       </c>
-      <c r="B277" s="1">
+      <c r="B277" s="2">
         <v>3.1599999999999999E-11</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A278">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A278" s="1">
         <v>111.2</v>
       </c>
-      <c r="B278" s="1">
+      <c r="B278" s="2">
         <v>2.92E-11</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A279">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A279" s="1">
         <v>111.6</v>
       </c>
-      <c r="B279" s="1">
+      <c r="B279" s="2">
         <v>2.96E-11</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A280">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A280" s="1">
         <v>112</v>
       </c>
-      <c r="B280" s="1">
+      <c r="B280" s="2">
         <v>3.12E-11</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A281">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A281" s="1">
         <v>112.4</v>
       </c>
-      <c r="B281" s="1">
+      <c r="B281" s="2">
         <v>3.1100000000000001E-11</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A282">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A282" s="1">
         <v>112.8</v>
       </c>
-      <c r="B282" s="1">
+      <c r="B282" s="2">
         <v>3.1100000000000001E-11</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A283">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A283" s="1">
         <v>113.2</v>
       </c>
-      <c r="B283" s="1">
+      <c r="B283" s="2">
         <v>2.9E-11</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A284">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A284" s="1">
         <v>113.6</v>
       </c>
-      <c r="B284" s="1">
+      <c r="B284" s="2">
         <v>2.92E-11</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A285">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A285" s="1">
         <v>114</v>
       </c>
-      <c r="B285" s="1">
+      <c r="B285" s="2">
         <v>2.82E-11</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A286">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A286" s="1">
         <v>114.4</v>
       </c>
-      <c r="B286" s="1">
+      <c r="B286" s="2">
         <v>2.84E-11</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A287">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A287" s="1">
         <v>114.8</v>
       </c>
-      <c r="B287" s="1">
+      <c r="B287" s="2">
         <v>2.9699999999999998E-11</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A288">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A288" s="1">
         <v>115.2</v>
       </c>
-      <c r="B288" s="1">
+      <c r="B288" s="2">
         <v>2.9699999999999998E-11</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A289">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A289" s="1">
         <v>115.6</v>
       </c>
-      <c r="B289" s="1">
+      <c r="B289" s="2">
         <v>2.92E-11</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A290">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A290" s="1">
         <v>116</v>
       </c>
-      <c r="B290" s="1">
+      <c r="B290" s="2">
         <v>2.8699999999999998E-11</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A291">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A291" s="1">
         <v>116.4</v>
       </c>
-      <c r="B291" s="1">
+      <c r="B291" s="2">
         <v>2.8099999999999999E-11</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A292">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A292" s="1">
         <v>116.8</v>
       </c>
-      <c r="B292" s="1">
+      <c r="B292" s="2">
         <v>2.74E-11</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A293">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A293" s="1">
         <v>117.2</v>
       </c>
-      <c r="B293" s="1">
+      <c r="B293" s="2">
         <v>2.82E-11</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A294">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A294" s="1">
         <v>117.6</v>
       </c>
-      <c r="B294" s="1">
+      <c r="B294" s="2">
         <v>2.74E-11</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A295">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A295" s="1">
         <v>118</v>
       </c>
-      <c r="B295" s="1">
+      <c r="B295" s="2">
         <v>2.7899999999999999E-11</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A296">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A296" s="1">
         <v>118.4</v>
       </c>
-      <c r="B296" s="1">
+      <c r="B296" s="2">
         <v>2.6299999999999999E-11</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A297">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A297" s="1">
         <v>118.8</v>
       </c>
-      <c r="B297" s="1">
+      <c r="B297" s="2">
         <v>2.8299999999999999E-11</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A298">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A298" s="1">
         <v>119.2</v>
       </c>
-      <c r="B298" s="1">
+      <c r="B298" s="2">
         <v>2.8299999999999999E-11</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A299">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A299" s="1">
         <v>119.6</v>
       </c>
-      <c r="B299" s="1">
+      <c r="B299" s="2">
         <v>2.7299999999999999E-11</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A300">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A300" s="1">
         <v>120</v>
       </c>
-      <c r="B300" s="1">
+      <c r="B300" s="2">
         <v>2.5800000000000001E-11</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A301">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A301" s="1">
         <v>120.4</v>
       </c>
-      <c r="B301" s="1">
+      <c r="B301" s="2">
         <v>2.5099999999999999E-11</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A302">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A302" s="1">
         <v>120.8</v>
       </c>
-      <c r="B302" s="1">
+      <c r="B302" s="2">
         <v>2.5800000000000001E-11</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A303">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A303" s="1">
         <v>121.2</v>
       </c>
-      <c r="B303" s="1">
+      <c r="B303" s="2">
         <v>2.6299999999999999E-11</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A304">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A304" s="1">
         <v>121.6</v>
       </c>
-      <c r="B304" s="1">
+      <c r="B304" s="2">
         <v>2.6400000000000001E-11</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A305">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A305" s="1">
         <v>122</v>
       </c>
-      <c r="B305" s="1">
+      <c r="B305" s="2">
         <v>2.5000000000000001E-11</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A306">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A306" s="1">
         <v>122.4</v>
       </c>
-      <c r="B306" s="1">
+      <c r="B306" s="2">
         <v>2.4699999999999999E-11</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A307">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A307" s="1">
         <v>122.8</v>
       </c>
-      <c r="B307" s="1">
+      <c r="B307" s="2">
         <v>2.3800000000000001E-11</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A308">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A308" s="1">
         <v>123.2</v>
       </c>
-      <c r="B308" s="1">
+      <c r="B308" s="2">
         <v>2.4600000000000001E-11</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A309">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A309" s="1">
         <v>123.6</v>
       </c>
-      <c r="B309" s="1">
+      <c r="B309" s="2">
         <v>2.37E-11</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A310">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A310" s="1">
         <v>124</v>
       </c>
-      <c r="B310" s="1">
+      <c r="B310" s="2">
         <v>2.23E-11</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A311">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A311" s="1">
         <v>124.4</v>
       </c>
-      <c r="B311" s="1">
+      <c r="B311" s="2">
         <v>2.1399999999999998E-11</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A312">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A312" s="1">
         <v>124.8</v>
       </c>
-      <c r="B312" s="1">
+      <c r="B312" s="2">
         <v>2.4000000000000001E-11</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A313">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A313" s="1">
         <v>125.2</v>
       </c>
-      <c r="B313" s="1">
+      <c r="B313" s="2">
         <v>2.33E-11</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A314">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A314" s="1">
         <v>125.6</v>
       </c>
-      <c r="B314" s="1">
+      <c r="B314" s="2">
         <v>2.2600000000000001E-11</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A315">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A315" s="1">
         <v>126</v>
       </c>
-      <c r="B315" s="1">
+      <c r="B315" s="2">
         <v>2.23E-11</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A316">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A316" s="1">
         <v>126.4</v>
       </c>
-      <c r="B316" s="1">
+      <c r="B316" s="2">
         <v>2.21E-11</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A317">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A317" s="1">
         <v>126.8</v>
       </c>
-      <c r="B317" s="1">
+      <c r="B317" s="2">
         <v>2.3000000000000001E-11</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A318">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A318" s="1">
         <v>127.2</v>
       </c>
-      <c r="B318" s="1">
+      <c r="B318" s="2">
         <v>2.19E-11</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A319">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A319" s="1">
         <v>127.6</v>
       </c>
-      <c r="B319" s="1">
+      <c r="B319" s="2">
         <v>2.0399999999999999E-11</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A320">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A320" s="1">
         <v>128</v>
       </c>
-      <c r="B320" s="1">
+      <c r="B320" s="2">
         <v>1.99E-11</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A321">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A321" s="1">
         <v>128.4</v>
       </c>
-      <c r="B321" s="1">
+      <c r="B321" s="2">
         <v>1.9599999999999999E-11</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A322">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A322" s="1">
         <v>128.80000000000001</v>
       </c>
-      <c r="B322" s="1">
+      <c r="B322" s="2">
         <v>1.97E-11</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A323">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A323" s="1">
         <v>129.19999999999999</v>
       </c>
-      <c r="B323" s="1">
+      <c r="B323" s="2">
         <v>2.0199999999999999E-11</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A324">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A324" s="1">
         <v>129.6</v>
       </c>
-      <c r="B324" s="1">
+      <c r="B324" s="2">
         <v>1.9100000000000001E-11</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A325">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A325" s="1">
         <v>130</v>
       </c>
-      <c r="B325" s="1">
+      <c r="B325" s="2">
         <v>1.9399999999999999E-11</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A326">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A326" s="1">
         <v>130.4</v>
       </c>
-      <c r="B326" s="1">
+      <c r="B326" s="2">
         <v>1.9999999999999999E-11</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A327">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A327" s="1">
         <v>130.80000000000001</v>
       </c>
-      <c r="B327" s="1">
+      <c r="B327" s="2">
         <v>2.03E-11</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A328">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A328" s="1">
         <v>131.19999999999999</v>
       </c>
-      <c r="B328" s="1">
+      <c r="B328" s="2">
         <v>2.09E-11</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A329">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A329" s="1">
         <v>131.6</v>
       </c>
-      <c r="B329" s="1">
+      <c r="B329" s="2">
         <v>1.8799999999999999E-11</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A330">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A330" s="1">
         <v>132</v>
       </c>
-      <c r="B330" s="1">
+      <c r="B330" s="2">
         <v>1.8599999999999999E-11</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A331">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A331" s="1">
         <v>132.4</v>
       </c>
-      <c r="B331" s="1">
+      <c r="B331" s="2">
         <v>1.8500000000000001E-11</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A332">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A332" s="1">
         <v>132.80000000000001</v>
       </c>
-      <c r="B332" s="1">
+      <c r="B332" s="2">
         <v>1.9100000000000001E-11</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A333">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A333" s="1">
         <v>133.19999999999999</v>
       </c>
-      <c r="B333" s="1">
+      <c r="B333" s="2">
         <v>1.8700000000000001E-11</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A334">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A334" s="1">
         <v>133.6</v>
       </c>
-      <c r="B334" s="1">
+      <c r="B334" s="2">
         <v>1.9399999999999999E-11</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A335">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A335" s="1">
         <v>134</v>
       </c>
-      <c r="B335" s="1">
+      <c r="B335" s="2">
         <v>1.8599999999999999E-11</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A336">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A336" s="1">
         <v>134.4</v>
       </c>
-      <c r="B336" s="1">
+      <c r="B336" s="2">
         <v>1.8100000000000001E-11</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A337">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A337" s="1">
         <v>134.80000000000001</v>
       </c>
-      <c r="B337" s="1">
+      <c r="B337" s="2">
         <v>1.9199999999999999E-11</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A338">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A338" s="1">
         <v>135.19999999999999</v>
       </c>
-      <c r="B338" s="1">
+      <c r="B338" s="2">
         <v>1.9300000000000001E-11</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A339">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A339" s="1">
         <v>135.6</v>
       </c>
-      <c r="B339" s="1">
+      <c r="B339" s="2">
         <v>1.8799999999999999E-11</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A340">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A340" s="1">
         <v>136</v>
       </c>
-      <c r="B340" s="1">
+      <c r="B340" s="2">
         <v>1.7799999999999999E-11</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A341">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A341" s="1">
         <v>136.4</v>
       </c>
-      <c r="B341" s="1">
+      <c r="B341" s="2">
         <v>1.9300000000000001E-11</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A342">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A342" s="1">
         <v>136.80000000000001</v>
       </c>
-      <c r="B342" s="1">
+      <c r="B342" s="2">
         <v>1.8700000000000001E-11</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A343">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A343" s="1">
         <v>137.19999999999999</v>
       </c>
-      <c r="B343" s="1">
+      <c r="B343" s="2">
         <v>1.8700000000000001E-11</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A344">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A344" s="1">
         <v>137.6</v>
       </c>
-      <c r="B344" s="1">
+      <c r="B344" s="2">
         <v>1.8799999999999999E-11</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A345">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A345" s="1">
         <v>138</v>
       </c>
-      <c r="B345" s="1">
+      <c r="B345" s="2">
         <v>1.7700000000000001E-11</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A346">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A346" s="1">
         <v>138.4</v>
       </c>
-      <c r="B346" s="1">
+      <c r="B346" s="2">
         <v>1.8700000000000001E-11</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A347">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A347" s="1">
         <v>138.80000000000001</v>
       </c>
-      <c r="B347" s="1">
+      <c r="B347" s="2">
         <v>1.8100000000000001E-11</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A348">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A348" s="1">
         <v>139.19999999999999</v>
       </c>
-      <c r="B348" s="1">
+      <c r="B348" s="2">
         <v>1.64E-11</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A349">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A349" s="1">
         <v>139.6</v>
       </c>
-      <c r="B349" s="1">
+      <c r="B349" s="2">
         <v>1.58E-11</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A350">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A350" s="1">
         <v>140</v>
       </c>
-      <c r="B350" s="1">
+      <c r="B350" s="2">
         <v>1.7100000000000001E-11</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A351">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A351" s="1">
         <v>140.4</v>
       </c>
-      <c r="B351" s="1">
+      <c r="B351" s="2">
         <v>1.7300000000000001E-11</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A352">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A352" s="1">
         <v>140.80000000000001</v>
       </c>
-      <c r="B352" s="1">
+      <c r="B352" s="2">
         <v>1.6E-11</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A353">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A353" s="1">
         <v>141.19999999999999</v>
       </c>
-      <c r="B353" s="1">
+      <c r="B353" s="2">
         <v>1.5500000000000001E-11</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A354">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A354" s="1">
         <v>141.6</v>
       </c>
-      <c r="B354" s="1">
+      <c r="B354" s="2">
         <v>1.45E-11</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A355">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A355" s="1">
         <v>142</v>
       </c>
-      <c r="B355" s="1">
+      <c r="B355" s="2">
         <v>1.58E-11</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A356">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A356" s="1">
         <v>142.4</v>
       </c>
-      <c r="B356" s="1">
+      <c r="B356" s="2">
         <v>1.5300000000000001E-11</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A357">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A357" s="1">
         <v>142.80000000000001</v>
       </c>
-      <c r="B357" s="1">
+      <c r="B357" s="2">
         <v>1.41E-11</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A358">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A358" s="1">
         <v>143.19999999999999</v>
       </c>
-      <c r="B358" s="1">
+      <c r="B358" s="2">
         <v>1.45E-11</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A359">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A359" s="1">
         <v>143.6</v>
       </c>
-      <c r="B359" s="1">
+      <c r="B359" s="2">
         <v>1.38E-11</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A360">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A360" s="1">
         <v>144</v>
       </c>
-      <c r="B360" s="1">
+      <c r="B360" s="2">
         <v>1.38E-11</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A361">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A361" s="1">
         <v>144.4</v>
       </c>
-      <c r="B361" s="1">
+      <c r="B361" s="2">
         <v>1.54E-11</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A362">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A362" s="1">
         <v>144.80000000000001</v>
       </c>
-      <c r="B362" s="1">
+      <c r="B362" s="2">
         <v>1.5900000000000001E-11</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A363">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A363" s="1">
         <v>145.19999999999999</v>
       </c>
-      <c r="B363" s="1">
+      <c r="B363" s="2">
         <v>1.46E-11</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A364">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A364" s="1">
         <v>145.6</v>
       </c>
-      <c r="B364" s="1">
+      <c r="B364" s="2">
         <v>1.32E-11</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A365">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A365" s="1">
         <v>146</v>
       </c>
-      <c r="B365" s="1">
+      <c r="B365" s="2">
         <v>1.31E-11</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A366">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A366" s="1">
         <v>146.4</v>
       </c>
-      <c r="B366" s="1">
+      <c r="B366" s="2">
         <v>1.35E-11</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A367">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A367" s="1">
         <v>146.80000000000001</v>
       </c>
-      <c r="B367" s="1">
+      <c r="B367" s="2">
         <v>1.5300000000000001E-11</v>
       </c>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A368">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A368" s="1">
         <v>147.19999999999999</v>
       </c>
-      <c r="B368" s="1">
+      <c r="B368" s="2">
         <v>1.39E-11</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A369">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A369" s="1">
         <v>147.6</v>
       </c>
-      <c r="B369" s="1">
+      <c r="B369" s="2">
         <v>1.34E-11</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A370">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A370" s="1">
         <v>148</v>
       </c>
-      <c r="B370" s="1">
+      <c r="B370" s="2">
         <v>1.31E-11</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A371">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A371" s="1">
         <v>148.4</v>
       </c>
-      <c r="B371" s="1">
+      <c r="B371" s="2">
         <v>1.43E-11</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A372">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A372" s="1">
         <v>148.80000000000001</v>
       </c>
-      <c r="B372" s="1">
+      <c r="B372" s="2">
         <v>1.41E-11</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A373">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A373" s="1">
         <v>149.19999999999999</v>
       </c>
-      <c r="B373" s="1">
+      <c r="B373" s="2">
         <v>1.3E-11</v>
       </c>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A374">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A374" s="1">
         <v>149.6</v>
       </c>
-      <c r="B374" s="1">
+      <c r="B374" s="2">
         <v>1.4900000000000002E-11</v>
       </c>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A375">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A375" s="1">
         <v>150</v>
       </c>
-      <c r="B375" s="1">
+      <c r="B375" s="2">
         <v>1.35E-11</v>
       </c>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A376">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A376" s="1">
         <v>150.4</v>
       </c>
-      <c r="B376" s="1">
+      <c r="B376" s="2">
         <v>1.36E-11</v>
       </c>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A377">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A377" s="1">
         <v>150.80000000000001</v>
       </c>
-      <c r="B377" s="1">
+      <c r="B377" s="2">
         <v>1.36E-11</v>
       </c>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A378">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A378" s="1">
         <v>151.19999999999999</v>
       </c>
-      <c r="B378" s="1">
+      <c r="B378" s="2">
         <v>1.44E-11</v>
       </c>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A379">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A379" s="1">
         <v>151.6</v>
       </c>
-      <c r="B379" s="1">
+      <c r="B379" s="2">
         <v>1.37E-11</v>
       </c>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A380">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A380" s="1">
         <v>152</v>
       </c>
-      <c r="B380" s="1">
+      <c r="B380" s="2">
         <v>1.2100000000000001E-11</v>
       </c>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A381">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A381" s="1">
         <v>152.4</v>
       </c>
-      <c r="B381" s="1">
+      <c r="B381" s="2">
         <v>1.2200000000000001E-11</v>
       </c>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A382">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A382" s="1">
         <v>152.80000000000001</v>
       </c>
-      <c r="B382" s="1">
+      <c r="B382" s="2">
         <v>1.28E-11</v>
       </c>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A383">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A383" s="1">
         <v>153.19999999999999</v>
       </c>
-      <c r="B383" s="1">
+      <c r="B383" s="2">
         <v>1.46E-11</v>
       </c>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A384">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A384" s="1">
         <v>153.6</v>
       </c>
-      <c r="B384" s="1">
+      <c r="B384" s="2">
         <v>1.2100000000000001E-11</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A385">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A385" s="1">
         <v>154</v>
       </c>
-      <c r="B385" s="1">
+      <c r="B385" s="2">
         <v>1.1100000000000001E-11</v>
       </c>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A386">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A386" s="1">
         <v>154.4</v>
       </c>
-      <c r="B386" s="1">
+      <c r="B386" s="2">
         <v>1.2200000000000001E-11</v>
       </c>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A387">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A387" s="1">
         <v>154.80000000000001</v>
       </c>
-      <c r="B387" s="1">
+      <c r="B387" s="2">
         <v>1.31E-11</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A388">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A388" s="1">
         <v>155.19999999999999</v>
       </c>
-      <c r="B388" s="1">
+      <c r="B388" s="2">
         <v>1.48E-11</v>
       </c>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A389">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A389" s="1">
         <v>155.6</v>
       </c>
-      <c r="B389" s="1">
+      <c r="B389" s="2">
         <v>1.34E-11</v>
       </c>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A390">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A390" s="1">
         <v>156</v>
       </c>
-      <c r="B390" s="1">
+      <c r="B390" s="2">
         <v>1.0699999999999999E-11</v>
       </c>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A391">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A391" s="1">
         <v>156.4</v>
       </c>
-      <c r="B391" s="1">
+      <c r="B391" s="2">
         <v>1.0599999999999999E-11</v>
       </c>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A392">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A392" s="1">
         <v>156.80000000000001</v>
       </c>
-      <c r="B392" s="1">
+      <c r="B392" s="2">
         <v>1.37E-11</v>
       </c>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A393">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A393" s="1">
         <v>157.19999999999999</v>
       </c>
-      <c r="B393" s="1">
+      <c r="B393" s="2">
         <v>1.32E-11</v>
       </c>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A394">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A394" s="1">
         <v>157.6</v>
       </c>
-      <c r="B394" s="1">
+      <c r="B394" s="2">
         <v>1.0499999999999999E-11</v>
       </c>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A395">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A395" s="1">
         <v>158</v>
       </c>
-      <c r="B395" s="1">
+      <c r="B395" s="2">
         <v>1.0699999999999999E-11</v>
       </c>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A396">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A396" s="1">
         <v>158.4</v>
       </c>
-      <c r="B396" s="1">
+      <c r="B396" s="2">
         <v>9.9700000000000005E-12</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A397">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A397" s="1">
         <v>158.80000000000001</v>
       </c>
-      <c r="B397" s="1">
+      <c r="B397" s="2">
         <v>1.29E-11</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A398">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A398" s="1">
         <v>159.19999999999999</v>
       </c>
-      <c r="B398" s="1">
+      <c r="B398" s="2">
         <v>1.1100000000000001E-11</v>
       </c>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A399">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A399" s="1">
         <v>159.6</v>
       </c>
-      <c r="B399" s="1">
+      <c r="B399" s="2">
         <v>9.8899999999999993E-12</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A400">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A400" s="1">
         <v>160</v>
       </c>
-      <c r="B400" s="1">
+      <c r="B400" s="2">
         <v>1.0299999999999999E-11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>